<commit_message>
change webhook for generations exel files
</commit_message>
<xml_diff>
--- a/allPages/allPagesEN.xlsx
+++ b/allPages/allPagesEN.xlsx
@@ -11,7 +11,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="189">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Headlines</t>
+  </si>
+  <si>
+    <t>SEO Title</t>
+  </si>
+  <si>
+    <t>Keywords</t>
+  </si>
   <si>
     <t>Pages</t>
   </si>
@@ -25,6 +43,9 @@
     <t>x</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>Foreign Economic Activity, delivery and customs clearance services in Ukraine in Kiev, Lviv, Odessa</t>
   </si>
   <si>
@@ -88,9 +109,6 @@
     <t>http://localhost:3000/en/cost_of_opening_a_legal_entity_in_ukraine</t>
   </si>
   <si>
-    <t>["Cost of Opening a Legal Entity in Ukraine: Detailed Overview and Calculations"]</t>
-  </si>
-  <si>
     <t>Cost of Opening a Legal Entity in Ukraine: Detailed Overview and Calculations</t>
   </si>
   <si>
@@ -121,7 +139,7 @@
     <t>http://localhost:3000/en/bank_account_in_ukraine</t>
   </si>
   <si>
-    <t>["Opening and Maintaining Bank Accounts for Legal Entities in Ukraine"]</t>
+    <t>Opening and Maintaining Bank Accounts for Legal Entities in Ukraine</t>
   </si>
   <si>
     <t>Opening and Maintaining a Bank Account for Legal Entities in Ukraine: A complete guide</t>
@@ -133,7 +151,7 @@
     <t>http://localhost:3000/en/taxation_forms_in_ukraine</t>
   </si>
   <si>
-    <t>["Forms of Taxation in Ukraine: How to Choose the Optimal Tax Regime for Your Business"]</t>
+    <t>Forms of Taxation in Ukraine: How to Choose the Optimal Tax Regime for Your Business</t>
   </si>
   <si>
     <t>Forms of taxation in Ukraine: How to choose the right tax regime for your business</t>
@@ -148,7 +166,7 @@
     <t>http://localhost:3000/en/legal_address_in_ukraine</t>
   </si>
   <si>
-    <t>["Legal Address in Ukraine: An Important Solution for Your Business"]</t>
+    <t>Legal Address in Ukraine: An Important Solution for Your Business</t>
   </si>
   <si>
     <t>Legal Address in Ukraine: An Important Element for Your Business</t>
@@ -160,7 +178,7 @@
     <t>http://localhost:3000/en/main_forms_of_ownership_in_ukraine</t>
   </si>
   <si>
-    <t>["Forms of Ownership in Ukraine: What is Suitable in Your Case?"]</t>
+    <t>Forms of Ownership in Ukraine: What is Suitable in Your Case?</t>
   </si>
   <si>
     <t>Forms of Ownership in Ukraine: Everything You Need to Know</t>
@@ -172,7 +190,7 @@
     <t>http://localhost:3000/en/opening_a_company_in_ukraine</t>
   </si>
   <si>
-    <t>["Starting a company in Ukraine: A Complete Guide for Entrepreneurs"]</t>
+    <t>Starting a company in Ukraine: A Complete Guide for Entrepreneurs</t>
   </si>
   <si>
     <t>Starting a Legal Entity in Ukraine: Step by Step Guidance and Tips</t>
@@ -187,7 +205,7 @@
     <t>http://localhost:3000/en/trade_agent_in_ukraine</t>
   </si>
   <si>
-    <t>["Trade Agent in Ukraine: Your Partner in World Trade"]</t>
+    <t>Trade Agent in Ukraine: Your Partner in World Trade</t>
   </si>
   <si>
     <t>Trade Agent in Ukraine: Effective Support for your Foreign Trade Business</t>
@@ -199,7 +217,7 @@
     <t>http://localhost:3000/en/foreign_trade_consulting</t>
   </si>
   <si>
-    <t>["Foreign Trade Consulting: The Key to Successful International Trade"]</t>
+    <t>Foreign Trade Consulting: The Key to Successful International Trade</t>
   </si>
   <si>
     <t>Foreign Economic Activity Consulting: Expert Guidance on Foreign Economic Activity</t>
@@ -214,7 +232,7 @@
     <t>http://localhost:3000/en/multimodal_transportation</t>
   </si>
   <si>
-    <t>["Multimodal Transportation"]</t>
+    <t>Multimodal Transportation</t>
   </si>
   <si>
     <t>Multimodal Transportation: Optimizing Freight Transportation in Europe and the World</t>
@@ -253,7 +271,7 @@
     <t>http://localhost:3000/en/port_forwarding</t>
   </si>
   <si>
-    <t>["Port Forwarding in Ukraine: Your Way to Effective Logistics","Basic Port Forwarding Services "]</t>
+    <t xml:space="preserve">Port Forwarding in Ukraine: Your Way to Effective Logistics, Basic Port Forwarding Services </t>
   </si>
   <si>
     <t>Port Forwarding in Ukraine - Reliable Logistics of Your Cargoes</t>
@@ -265,7 +283,7 @@
     <t>http://localhost:3000/en/customs_brokerage_services_cost</t>
   </si>
   <si>
-    <t>["Cost of Customs Brokerage Services in Ukraine","What Affects the Cost of Customs Brokerage Services? ","Why Cooperation with a Customs Broker is Beneficial? ","Advantages of Our Services in Kiev, Odessa and Lviv ","Approximate Cost of Customs Brokerage Services"]</t>
+    <t>Cost of Customs Brokerage Services in Ukraine, What Affects the Cost of Customs Brokerage Services? , Why Cooperation with a Customs Broker is Beneficial? , Advantages of Our Services in Kiev, Odessa and Lviv , Approximate Cost of Customs Brokerage Services</t>
   </si>
   <si>
     <t>Cost of Customs Brokerage Services in Ukraine: Professional Assistance and Optimization of Foreign Economic Activity</t>
@@ -277,7 +295,7 @@
     <t>http://localhost:3000/en/customs_broker</t>
   </si>
   <si>
-    <t>["Customs broker: Your reliable partner in Kiev, Odessa and Lviv","Who is a Customs Broker?","Customs broker services ","Why choose us?","Customs broker in Kiev","Customs broker in Odessa","Customs broker in Lviv","Advantages of working with us "]</t>
+    <t xml:space="preserve">Customs broker: Your reliable partner in Kiev, Odessa and Lviv, Who is a Customs Broker?, Customs broker services , Why choose us?, Customs broker in Kiev, Customs broker in Odessa, Customs broker in Lviv, Advantages of working with us </t>
   </si>
   <si>
     <t>Customs broker Ukraine: Professional services in Kiev, Odessa and Lviv</t>
@@ -328,9 +346,6 @@
     <t>http://localhost:3000/en/privacy_policy</t>
   </si>
   <si>
-    <t>["Privacy Policy"]</t>
-  </si>
-  <si>
     <t>Privacy Policy</t>
   </si>
   <si>
@@ -349,7 +364,7 @@
     <t>http://localhost:3000/en/customs_clearance</t>
   </si>
   <si>
-    <t>["Customs clearance in Ukraine: Fast, Reliable, Professional "]</t>
+    <t xml:space="preserve">Customs clearance in Ukraine: Fast, Reliable, Professional </t>
   </si>
   <si>
     <t>Professional Customs Clearance in Ukraine: Fast and Reliable</t>
@@ -361,7 +376,7 @@
     <t>http://localhost:3000/en/container_delivery</t>
   </si>
   <si>
-    <t>["Sea Container Transportation: Reliable and Economical","Advantages of sea container transportation "]</t>
+    <t xml:space="preserve">Sea Container Transportation: Reliable and Economical, Advantages of sea container transportation </t>
   </si>
   <si>
     <t>Sea Container Transportation to Ukraine: Reliable and Economical</t>
@@ -373,7 +388,7 @@
     <t>http://localhost:3000/en/truck_delivery</t>
   </si>
   <si>
-    <t>["Road transportation"]</t>
+    <t>Road transportation</t>
   </si>
   <si>
     <t>Trucking: Reliable and Efficient Transportation of Your Cargo</t>
@@ -400,7 +415,7 @@
     <t>http://localhost:3000/en/sea_container_freight_rate</t>
   </si>
   <si>
-    <t>["Cost of Container Transportation by Sea"]</t>
+    <t>Cost of Container Transportation by Sea</t>
   </si>
   <si>
     <t>Cost of Container Transportation by Sea: Reliable and Competitive Rates</t>
@@ -412,7 +427,7 @@
     <t>http://localhost:3000/en/container_freight_rate</t>
   </si>
   <si>
-    <t>["Container Freight: Key Aspects and Freight Rate"]</t>
+    <t>Container Freight: Key Aspects and Freight Rate</t>
   </si>
   <si>
     <t>Container Freight: Exact prices and flexible conditions for freight transportation</t>
@@ -463,7 +478,7 @@
     <t>http://localhost:3000/en/blog/the-economics-of-low-cost-delivery-services</t>
   </si>
   <si>
-    <t>["Low-cost air cargo delivery to Ukraine.","Cost reduction ","Increase in revenues "]</t>
+    <t xml:space="preserve">Low-cost air cargo delivery to Ukraine., Cost reduction , Increase in revenues </t>
   </si>
   <si>
     <t>The economics of low-cost delivery: how airlines are reducing costs and increasing revenues.</t>
@@ -478,9 +493,6 @@
     <t>http://localhost:3000/en/blog/methods-of-transportation-containers-from-china-to-ukraine</t>
   </si>
   <si>
-    <t>["Ways of transportation of containers from China to Ukraine"]</t>
-  </si>
-  <si>
     <t>Ways of transportation of containers from China to Ukraine</t>
   </si>
   <si>
@@ -493,7 +505,7 @@
     <t>http://localhost:3000/en/blog/how-to-write-an-inquiry-to-a-chinese-supplier</t>
   </si>
   <si>
-    <t>["How to write a request to a Chinese supplier of goods?"]</t>
+    <t>How to write a request to a Chinese supplier of goods?</t>
   </si>
   <si>
     <t>How to write a inquiry to a Chinese supplier of goods?</t>
@@ -508,7 +520,7 @@
     <t>http://localhost:3000/en/blog/searching-for-suppliers-in-china</t>
   </si>
   <si>
-    <t>["Searching for suppliers in China"]</t>
+    <t>Searching for suppliers in China</t>
   </si>
   <si>
     <t>Search for suppliers in China</t>
@@ -942,729 +954,786 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F56"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E14" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F14" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F15" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C16" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E17" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F17" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E18" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>73</v>
       </c>
       <c r="E19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F19" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C20" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F20" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F21" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C22" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E22" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F22" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C23" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E23" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F23" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B24" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C24" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
+        <v>94</v>
       </c>
       <c r="E24" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F24" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B25" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C25" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F25" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C26" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
       </c>
       <c r="E26" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F26" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B27" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C27" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F27" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B28" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C28" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>105</v>
+        <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F28" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B29" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C29" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D29" t="s">
+        <v>111</v>
       </c>
       <c r="E29" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F29" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B30" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C30" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>112</v>
+        <v>10</v>
       </c>
       <c r="E30" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F30" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B31" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C31" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E31" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F31" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B32" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C32" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D32" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E32" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F32" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="B33" t="s">
         <v>124</v>
       </c>
       <c r="C33" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D33" t="s">
+        <v>125</v>
       </c>
       <c r="E33" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F33" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>128</v>
+      </c>
+      <c r="B34" t="s">
+        <v>129</v>
+      </c>
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" t="s">
+        <v>130</v>
+      </c>
+      <c r="F34" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>65</v>
-      </c>
-      <c r="B36" t="s">
-        <v>128</v>
-      </c>
-      <c r="C36" t="s">
-        <v>3</v>
-      </c>
-      <c r="D36" t="s">
-        <v>129</v>
-      </c>
-      <c r="E36" t="s">
-        <v>130</v>
-      </c>
-      <c r="F36" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C37" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D37" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E37" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F37" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B38" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C38" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D38" t="s">
+        <v>138</v>
       </c>
       <c r="E38" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F38" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B39" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C39" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D39" t="s">
+        <v>10</v>
       </c>
       <c r="E39" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F39" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>142</v>
+        <v>76</v>
       </c>
       <c r="B40" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C40" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D40" t="s">
+        <v>10</v>
       </c>
       <c r="E40" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F40" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>148</v>
+      </c>
+      <c r="C41" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" t="s">
+        <v>149</v>
+      </c>
+      <c r="F41" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>148</v>
-      </c>
-      <c r="B45" t="s">
-        <v>149</v>
-      </c>
-      <c r="C45" t="s">
-        <v>3</v>
-      </c>
-      <c r="D45" t="s">
-        <v>150</v>
-      </c>
-      <c r="E45" t="s">
-        <v>151</v>
-      </c>
-      <c r="F45" t="s">
         <v>152</v>
       </c>
     </row>
@@ -1676,7 +1745,7 @@
         <v>154</v>
       </c>
       <c r="C46" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D46" t="s">
         <v>155</v>
@@ -1696,126 +1765,161 @@
         <v>159</v>
       </c>
       <c r="C47" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D47" t="s">
         <v>160</v>
       </c>
       <c r="E47" t="s">
+        <v>160</v>
+      </c>
+      <c r="F47" t="s">
         <v>161</v>
-      </c>
-      <c r="F47" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>162</v>
+      </c>
+      <c r="B48" t="s">
         <v>163</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" t="s">
         <v>164</v>
       </c>
-      <c r="C48" t="s">
-        <v>3</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>165</v>
       </c>
-      <c r="E48" t="s">
+      <c r="F48" t="s">
         <v>166</v>
       </c>
-      <c r="F48" t="s">
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="B49" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" t="s">
+        <v>169</v>
+      </c>
+      <c r="E49" t="s">
+        <v>170</v>
+      </c>
+      <c r="F49" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>169</v>
-      </c>
-      <c r="B51" t="s">
-        <v>170</v>
-      </c>
-      <c r="C51" t="s">
-        <v>3</v>
-      </c>
-      <c r="E51" t="s">
-        <v>171</v>
-      </c>
-      <c r="F51" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B52" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C52" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D52" t="s">
+        <v>10</v>
       </c>
       <c r="E52" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F52" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B53" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C53" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D53" t="s">
+        <v>10</v>
       </c>
       <c r="E53" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F53" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B54" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C54" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D54" t="s">
+        <v>10</v>
       </c>
       <c r="E54" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F54" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B55" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C55" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D55" t="s">
+        <v>10</v>
       </c>
       <c r="E55" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F55" t="s">
-        <v>184</v>
+        <v>185</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>173</v>
+      </c>
+      <c r="B56" t="s">
+        <v>186</v>
+      </c>
+      <c r="C56" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" t="s">
+        <v>10</v>
+      </c>
+      <c r="E56" t="s">
+        <v>187</v>
+      </c>
+      <c r="F56" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change xlsx webhook generations
</commit_message>
<xml_diff>
--- a/allPages/allPagesEN.xlsx
+++ b/allPages/allPagesEN.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="217">
   <si>
     <t>Date</t>
   </si>
@@ -22,12 +22,15 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Headlines</t>
+    <t>Title</t>
   </si>
   <si>
     <t>SEO Title</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
     <t>Keywords</t>
   </si>
   <si>
@@ -43,12 +46,12 @@
     <t>x</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Foreign Economic Activity, delivery and customs clearance services in Ukraine in Kiev, Lviv, Odessa</t>
   </si>
   <si>
+    <t>Professional trade agent in Ukraine, assistance in import and export operations in Ukraine. We provide advice, support in customs clearance and logistics. Trust our experience for successful export and import of goods and services.</t>
+  </si>
+  <si>
     <t>trade intermediary, foreign trade agent, export consultant, import broker, foreign trade consultancy, world trade, international business, trade with Ukraine, foreign economic activity.</t>
   </si>
   <si>
@@ -61,6 +64,9 @@
     <t>Customs broker and customs clearance in Ukraine Kiev, Odessa, Lviv, Ukraine</t>
   </si>
   <si>
+    <t>Customs broker for customs clearance in Kiev, Odessa or Lviv</t>
+  </si>
+  <si>
     <t>customs clearance Kiev, customs clearance services Lviv, customs broker Odessa, calculation of customs payments, cargo escort, customs documents, customs services</t>
   </si>
   <si>
@@ -70,6 +76,9 @@
     <t>Maritime container transportation and cargo delivery from USA and China to Ukraine</t>
   </si>
   <si>
+    <t>Need sea container transportation for cargo delivery from USA and China to Ukraine? We provide safe and timely delivery of goods by sea, guaranteeing full control and reliability at every stage of transportation.</t>
+  </si>
+  <si>
     <t>cargo delivery from USA to Ukraine, sea container transportation, delivery from China to Ukraine, container transportation Ukraine, sea delivery from China, international sea transportation</t>
   </si>
   <si>
@@ -79,6 +88,9 @@
     <t>Air delivery and air cargo transportation to Ukraine: fast and reliable</t>
   </si>
   <si>
+    <t>Looking for efficient solutions for air delivery and air cargo transportation to Ukraine? We offer fast, reliable and safe air transportation.</t>
+  </si>
+  <si>
     <t>air cargo transportation Ukraine, air delivery to Ukraine, international air delivery, transportation of cargo by air, air logistics Ukraine, express air delivery, air freight, air cargo transportation, air logistics, air cargo transportation, air transportation from China, air transportation to Europe, air cargo delivery, air freight, air transportation of dangerous goods</t>
   </si>
   <si>
@@ -88,6 +100,9 @@
     <t>Auto transportation and cargo delivery from Europe: fast and safe solutions</t>
   </si>
   <si>
+    <t>Need auto transportation and cargo delivery from Europe to Ukraine? Our company offers fast and safe solutions for auto shipping of any cargo, providing efficiency and reliability at every stage of transportation of your cargo with us.</t>
+  </si>
+  <si>
     <t>auto transportation from Europe, delivery of goods by auto transport, international auto delivery, transportation of goods from Europe, auto logistics Europe, delivery of goods by auto transport.</t>
   </si>
   <si>
@@ -100,6 +115,9 @@
     <t>Useful materials on customs clearance and cargo delivery: tips and instructions</t>
   </si>
   <si>
+    <t>Discover useful materials on customs clearance and shipping.</t>
+  </si>
+  <si>
     <t>customs clearance, shipping instructions, logistics and customs clearance, successful cargo delivery, how to deliver cargo through customs</t>
   </si>
   <si>
@@ -112,6 +130,9 @@
     <t>Cost of Opening a Legal Entity in Ukraine: Detailed Overview and Calculations</t>
   </si>
   <si>
+    <t>Find out about the cost of opening a legal entity in Ukraine. Our review provides a detailed overview and calculations to estimate the initial costs of registering a company in Ukraine.</t>
+  </si>
+  <si>
     <t>Establishing a company in Ukraine, registration of a legal entity, the cost of opening a company, the cost of registering a business, the cost of a legal entity, the budget for registering a company</t>
   </si>
   <si>
@@ -121,6 +142,9 @@
     <t>Effective Personnel Search in Ukraine: Professional HR Solutions</t>
   </si>
   <si>
+    <t>Are you looking for a reliable partner for staff search and recruitment in Ukraine? Our company provides professional HR solutions to help you successfully find qualified employees. Trust us to optimize the recruitment process and build human resources potential in your company.</t>
+  </si>
+  <si>
     <t>recruitment, recruiting in Ukraine, HR-services, recruitment agency, employment in Ukraine, personnel management, search for specialists, personnel consulting, HR-consulting, personal resources of Ukraine</t>
   </si>
   <si>
@@ -130,6 +154,9 @@
     <t>Tax Reporting in Ukraine: Detailed Overview and Rules of Reporting Preparation</t>
   </si>
   <si>
+    <t>Find out everything about tax reporting in Ukraine. Our experts provide a detailed overview, rules and tips on how to properly prepare tax reports for your company.</t>
+  </si>
+  <si>
     <t>tax reporting, tax returns, tax liabilities, tax rates, tax regulations, tax legislation, accounting and taxes, tax changes, tax obligations, tax administration</t>
   </si>
   <si>
@@ -139,24 +166,24 @@
     <t>http://localhost:3000/en/bank_account_in_ukraine</t>
   </si>
   <si>
-    <t>Opening and Maintaining Bank Accounts for Legal Entities in Ukraine</t>
-  </si>
-  <si>
     <t>Opening and Maintaining a Bank Account for Legal Entities in Ukraine: A complete guide</t>
   </si>
   <si>
+    <t>Opening and maintaining a bank account for legal entities in Ukraine is an important stage in the financial activity of your company. A complete guide to opening and managing a bank account to ensure the financial stability of your company.</t>
+  </si>
+  <si>
     <t>business account, corporate account, banking services for companies, banking services for legal entities, financial activity of organizations, account in the bank of Ukraine, opening an account for the company, banking services for companies</t>
   </si>
   <si>
     <t>http://localhost:3000/en/taxation_forms_in_ukraine</t>
   </si>
   <si>
-    <t>Forms of Taxation in Ukraine: How to Choose the Optimal Tax Regime for Your Business</t>
-  </si>
-  <si>
     <t>Forms of taxation in Ukraine: How to choose the right tax regime for your business</t>
   </si>
   <si>
+    <t>Find out about the different forms of taxation in Ukraine. Tax obligations, benefits and opportunities provided by different tax regimes. Choose the most suitable tax regime for your business.</t>
+  </si>
+  <si>
     <t>tax regimes, tax system, tax liabilities, tax rate, tax benefits, tax payment, tax optimization, tax regime for business, tax accounting, fiscal policy, tax reporting, tax obligations</t>
   </si>
   <si>
@@ -166,36 +193,36 @@
     <t>http://localhost:3000/en/legal_address_in_ukraine</t>
   </si>
   <si>
-    <t>Legal Address in Ukraine: An Important Solution for Your Business</t>
-  </si>
-  <si>
     <t>Legal Address in Ukraine: An Important Element for Your Business</t>
   </si>
   <si>
+    <t>Discover how to choose and register a legal address for your business in Ukraine. Let's consider how to choose and register a legal address and what important aspects should be taken into account.</t>
+  </si>
+  <si>
     <t>address of incorporation in Ukraine, registration of legal address, tax address, office space, legal registration, choice of location, company reputation, tax liabilities</t>
   </si>
   <si>
     <t>http://localhost:3000/en/main_forms_of_ownership_in_ukraine</t>
   </si>
   <si>
-    <t>Forms of Ownership in Ukraine: What is Suitable in Your Case?</t>
-  </si>
-  <si>
     <t>Forms of Ownership in Ukraine: Everything You Need to Know</t>
   </si>
   <si>
+    <t>Learn about the various forms of ownership in Ukraine. Let's explore ownership options, rules and procedures for their registration, and talk about the most suitable form of ownership for your business or investment in Ukraine.</t>
+  </si>
+  <si>
     <t>property in Ukraine, property registration, ownership rules, forms of ownership in business, ownership of real estate, property and taxes, types of ownership</t>
   </si>
   <si>
     <t>http://localhost:3000/en/opening_a_company_in_ukraine</t>
   </si>
   <si>
-    <t>Starting a company in Ukraine: A Complete Guide for Entrepreneurs</t>
-  </si>
-  <si>
     <t>Starting a Legal Entity in Ukraine: Step by Step Guidance and Tips</t>
   </si>
   <si>
+    <t>Do you want to open a legal entity in Ukraine? Our detailed guide will tell you how to do it. Learn about all stages of business registration, necessary documents, tax aspects and other important nuances. We provide useful tips and instructions for a successful start of your business in Ukraine.</t>
+  </si>
+  <si>
     <t>company registration, business in Ukraine, startup in Ukraine, entrepreneurship in Ukraine, establish a company, tax legislation, registration rules, documents for business</t>
   </si>
   <si>
@@ -205,9 +232,6 @@
     <t>http://localhost:3000/en/trade_agent_in_ukraine</t>
   </si>
   <si>
-    <t>Trade Agent in Ukraine: Your Partner in World Trade</t>
-  </si>
-  <si>
     <t>Trade Agent in Ukraine: Effective Support for your Foreign Trade Business</t>
   </si>
   <si>
@@ -217,12 +241,12 @@
     <t>http://localhost:3000/en/foreign_trade_consulting</t>
   </si>
   <si>
-    <t>Foreign Trade Consulting: The Key to Successful International Trade</t>
-  </si>
-  <si>
     <t>Foreign Economic Activity Consulting: Expert Guidance on Foreign Economic Activity</t>
   </si>
   <si>
+    <t>Get professional foreign trade consultations from experts in the field of foreign economic activity. Our consultants will help you understand complex issues of import and export, customs clearance and many other aspects of international trade. Ensure the success of your business abroad with our help.</t>
+  </si>
+  <si>
     <t>Foreign Economic Activity Consulting, Foreign Economic Activity Services, export-import consulting, customs consulting, international trade, export procedures, import regulations, Foreign Economic Expert, foreign economic activity</t>
   </si>
   <si>
@@ -232,12 +256,12 @@
     <t>http://localhost:3000/en/multimodal_transportation</t>
   </si>
   <si>
-    <t>Multimodal Transportation</t>
-  </si>
-  <si>
     <t>Multimodal Transportation: Optimizing Freight Transportation in Europe and the World</t>
   </si>
   <si>
+    <t>Multimodal transportation: global logistics in one solution. Save time and money by choosing the optimal transportation combinations for your shipment. Our multimodal solutions ensure reliable and efficient delivery.</t>
+  </si>
+  <si>
     <t>multimodal logistics, combined transport, multimodal transportation, global multimodal solutions, freight optimization, multimodal transportation in Europe, multimodal freight transportation, multimodal transportation within the country, multimodal delivery, multimodal transport</t>
   </si>
   <si>
@@ -250,6 +274,9 @@
     <t>Air Freight Costs: How to Calculate and Optimize Your Expenses</t>
   </si>
   <si>
+    <t>Learn how to calculate and optimize air freight costs. Effective strategies and tips to reduce air freight transportation costs. Plan your logistics operations smartly and save money with our help.</t>
+  </si>
+  <si>
     <t>air freight costs, air freight rates, air freight rates, air freight prices, air freight costs, air freight costs, air freight costs, budget for air freight, air freight savings, air freight costs</t>
   </si>
   <si>
@@ -262,6 +289,9 @@
     <t>Cargo delivery from Europe: Efficient Logistics for Your Business</t>
   </si>
   <si>
+    <t>Cargo delivery from Europe to Ukraine: your way to global trade. We provide reliable and efficient logistics for shipments from Europe. Find out how we simplify your business and make international shipments worry-free.</t>
+  </si>
+  <si>
     <t>ukraine, international delivery from Europe, logistics of cargoes from Europe, import from Europe, export to Europe, cargo transportation to Europe, transportation of goods from Europe, European deliveries, transportation of cargoes through Europe</t>
   </si>
   <si>
@@ -271,36 +301,36 @@
     <t>http://localhost:3000/en/port_forwarding</t>
   </si>
   <si>
-    <t xml:space="preserve">Port Forwarding in Ukraine: Your Way to Effective Logistics, Basic Port Forwarding Services </t>
-  </si>
-  <si>
     <t>Port Forwarding in Ukraine - Reliable Logistics of Your Cargoes</t>
   </si>
   <si>
+    <t xml:space="preserve">Port forwarding of cargoes in Odessa, Yuzhny, Chernomorsk and other ports of Ukraine. We will provide a full cycle of logistics: from documentary support to door-to-door delivery of cargo. </t>
+  </si>
+  <si>
     <t>sea freight forwarding, port services, port freight forwarding, port logistics, port cargo handling, marine terminals, port infrastructure, port cargo, sea transportation</t>
   </si>
   <si>
     <t>http://localhost:3000/en/customs_brokerage_services_cost</t>
   </si>
   <si>
-    <t>Cost of Customs Brokerage Services in Ukraine, What Affects the Cost of Customs Brokerage Services? , Why Cooperation with a Customs Broker is Beneficial? , Advantages of Our Services in Kiev, Odessa and Lviv , Approximate Cost of Customs Brokerage Services</t>
-  </si>
-  <si>
     <t>Cost of Customs Brokerage Services in Ukraine: Professional Assistance and Optimization of Foreign Economic Activity</t>
   </si>
   <si>
+    <t>How much does the service of a customs broker in Ukraine cost. Professional customs brokers in Kiev, Odessa and Lviv will help you quickly and efficiently process your shipments, saving you time and money.</t>
+  </si>
+  <si>
     <t>услуги таможенного брокера, стоимость таможенного брокера, таможенный брокер Киев, таможенный брокер Одесса, таможенный брокер Львов, услуги таможенного оформления, стоимость таможенных услуг, таможенное оформление грузов, таможенные брокеры Украина</t>
   </si>
   <si>
     <t>http://localhost:3000/en/customs_broker</t>
   </si>
   <si>
-    <t xml:space="preserve">Customs broker: Your reliable partner in Kiev, Odessa and Lviv, Who is a Customs Broker?, Customs broker services , Why choose us?, Customs broker in Kiev, Customs broker in Odessa, Customs broker in Lviv, Advantages of working with us </t>
-  </si>
-  <si>
     <t>Customs broker Ukraine: Professional services in Kiev, Odessa and Lviv</t>
   </si>
   <si>
+    <t>Professional services of customs broker in Kiev, Odessa and Lviv. Fast and high-quality customs clearance of cargo. Individual approach and high level of service.</t>
+  </si>
+  <si>
     <t>customs broker Ukraine, customs brokerage services, customs clearance, customs broker Kiev, customs broker Odessa, customs broker Lviv, customs services, international trade, import and export, customs declaration, brokerage services</t>
   </si>
   <si>
@@ -313,6 +343,9 @@
     <t>Frequently Asked Questions (FAQs)</t>
   </si>
   <si>
+    <t>Our Frequently Asked Questions (FAQs) are your source for answers to the most important questions about shipping and customs clearance. Clear your doubts and learn more about our services. Your clarity is our priority.</t>
+  </si>
+  <si>
     <t>FAQ Questions and Answers, Customer Information, Explanation of Services, Typical Questions, User Guide, Frequent Requests, Detailed Answers, Help and Tips, Customer Support</t>
   </si>
   <si>
@@ -322,6 +355,9 @@
     <t>Help &amp; Support: Your Guide to the World of Shipping and Customs Clearance</t>
   </si>
   <si>
+    <t>Our experts are here to help you every step of the way with shipping and customs clearance. Visit our Help page for answers to your questions and support contacts. Your comfort and satisfaction is our primary goal.</t>
+  </si>
+  <si>
     <t>customer service, customer support, customer assistance, customer help, frequently asked questions, customer service contacts, customer support, feedback, shipping assistance, customer counseling, technical support</t>
   </si>
   <si>
@@ -331,6 +367,9 @@
     <t>Cookies</t>
   </si>
   <si>
+    <t>Learn how we use cookies to improve your experience on our website. Our cookies help us analyze and optimize our shipping and customs services. We value your transparency and comfort in your online interaction with us.</t>
+  </si>
+  <si>
     <t>05.10.23</t>
   </si>
   <si>
@@ -340,6 +379,9 @@
     <t>Terms of Use</t>
   </si>
   <si>
+    <t>Our Terms of Use are your map to safe and secure shipping and customs clearance. Read our terms and conditions before using our services. Your safety and satisfaction is our priority.</t>
+  </si>
+  <si>
     <t>terms of use, terms of service, terms of use, terms of use policy, terms of use agreement, terms of use, terms of service, terms of service agreement, terms of use of the website, user agreement, terms of security, terms of security, terms of delivery, customs clearance agreement, terms of data processing</t>
   </si>
   <si>
@@ -349,51 +391,60 @@
     <t>Privacy Policy</t>
   </si>
   <si>
+    <t>Our Privacy Policy is your guarantee of transparency and security. We care about your privacy in the world of shipping and customs clearance. Find out how we protect your personal information. Your privacy is our priority</t>
+  </si>
+  <si>
     <t>Data privacy, personal data protection, personal data processing, website privacy policy, consent to data processing, data protection regulations, GDPR, data protection, information security, data protection assurance, customer privacy policy</t>
   </si>
   <si>
     <t>http://localhost:3000/en/about_us</t>
   </si>
   <si>
+    <t>About us</t>
+  </si>
+  <si>
     <t>About Us: Trans-Hope, Your Reliable Partner in Shipping and Customs Clearance</t>
   </si>
   <si>
-    <t>About us</t>
+    <t>Trans-Hope, Your Reliable Partner in Delivery and Customs clearance of cargo by the following types of transport: Air transportation, Auto cargo delivery, Sea container transportation, Customs clearance of cargo. Kyiv, Ukraine</t>
   </si>
   <si>
     <t>http://localhost:3000/en/customs_clearance</t>
   </si>
   <si>
-    <t xml:space="preserve">Customs clearance in Ukraine: Fast, Reliable, Professional </t>
+    <t>Customs clearance in Ukraine</t>
   </si>
   <si>
     <t>Professional Customs Clearance in Ukraine: Fast and Reliable</t>
   </si>
   <si>
+    <t>Customs clearance services for business in Ukraine in Kiev, Odessa, Lviv: fast and accurate execution of documents, calculation of payments, cargo support. Reliability and professionalism guaranteed!</t>
+  </si>
+  <si>
     <t>customs clearance, customs clearance services Ukraine, customs broker Kiev, customs payments calculation, cargo escort, customs documents, customs services Odessa</t>
   </si>
   <si>
     <t>http://localhost:3000/en/container_delivery</t>
   </si>
   <si>
-    <t xml:space="preserve">Sea Container Transportation: Reliable and Economical, Advantages of sea container transportation </t>
-  </si>
-  <si>
     <t>Sea Container Transportation to Ukraine: Reliable and Economical</t>
   </si>
   <si>
+    <t>Sea container transportation to Ukraine. Full range of services: from consulting and booking, to door-to-door delivery.</t>
+  </si>
+  <si>
     <t>sea container transportations, sea transportations to Ukraine, sea logistics, container transportations, sea freight, international sea transportations, container sea transportations, sea transport, container transportations by sea, sea forwarding, sea lines, sea transportations of goods, sea delivery, sea freight transportations, container logistics, sea transportation, sea freight services.</t>
   </si>
   <si>
     <t>http://localhost:3000/en/truck_delivery</t>
   </si>
   <si>
-    <t>Road transportation</t>
-  </si>
-  <si>
     <t>Trucking: Reliable and Efficient Transportation of Your Cargo</t>
   </si>
   <si>
+    <t>Auto transportation: reliable cargo delivery in Ukraine and European countries. We offer fast and efficient logistics for your business. Entrust us with the transportation of your cargo and be sure of the reliability of our services. Get a smooth solution for transportation of your cargo with us.</t>
+  </si>
+  <si>
     <t>Road Trucking, Road Freight, Road Freight Logistics, Road Freight Logistics, Road Freight Trucks, Road Freight Services, Road Freight Services, Road Freight Delivery, Road Freight Delivery, Road Freight Transportation, Road Freight Services, Road Freight Logistics, Road Freight, Road Freight, Road Freight Logistics Services, Road Freight Trucking, Road Freight Trucks, Road Freight Vans, Professional Road Freight Services</t>
   </si>
   <si>
@@ -406,6 +457,9 @@
     <t>Air transportation: fast, reliable and efficient</t>
   </si>
   <si>
+    <t>Air freight: fast delivery, global coverage and reliability. We ship worldwide in the shortest possible time. Find out how air freight can improve your business today.</t>
+  </si>
+  <si>
     <t>Air transportation, Air cargo transportation, International air transportation, Air cargo transportation, Air cargo transportation, Air cargo logistics, Air freight, Air cargo transportation, Air logistics, Air cargo transportation, Air cargo transportation, Air transportation from China, Air transportation to Europe, Air cargo transportation, Air cargo transportation, Air cargo transportation, Air transportation of dangerous goods</t>
   </si>
   <si>
@@ -415,24 +469,24 @@
     <t>http://localhost:3000/en/sea_container_freight_rate</t>
   </si>
   <si>
-    <t>Cost of Container Transportation by Sea</t>
-  </si>
-  <si>
     <t>Cost of Container Transportation by Sea: Reliable and Competitive Rates</t>
   </si>
   <si>
+    <t xml:space="preserve">Find out about the cost of shipping a container by sea. Our competitive rates ensure reliable and efficient delivery of your shipment anywhere in the world. We offer transparent pricing and high quality service for ocean freight transportation. </t>
+  </si>
+  <si>
     <t>price of sea transportation of containers, tariffs for sea transportation, cost of transportation by sea, rates for transportation by sea container, tariffs for container transportation</t>
   </si>
   <si>
     <t>http://localhost:3000/en/container_freight_rate</t>
   </si>
   <si>
-    <t>Container Freight: Key Aspects and Freight Rate</t>
-  </si>
-  <si>
     <t>Container Freight: Exact prices and flexible conditions for freight transportation</t>
   </si>
   <si>
+    <t>Find out the current shipping container freight prices and the benefits of our shipping services. We provide reliable and competitive container freight rates, allowing you to optimize your budget and ensure the safe delivery of your shipments worldwide.</t>
+  </si>
+  <si>
     <t>sea container freight rates, container freight rates, container freight tariffs, sea freight prices, freight tariffs</t>
   </si>
   <si>
@@ -442,6 +496,9 @@
     <t>Intermodal Transportation: Efficiency and Reliability in Global Logistics</t>
   </si>
   <si>
+    <t>Intermodal transportation: the optimal combination of different modes of transportation for efficient delivery of goods. Our intermodal solutions provide reliability and flexibility in global logistics. Find out how you can save on transportation costs by choosing our delivery system.</t>
+  </si>
+  <si>
     <t>intermodal freight transportation, multimodal transportation, combined transportation, transportation of goods by different modes of transportation</t>
   </si>
   <si>
@@ -451,6 +508,9 @@
     <t>Costs for Customs Brokerage Services: Transparency and Efficiency, Kyiv Ukraine</t>
   </si>
   <si>
+    <t>Find out what are the prices for customs broker services in Kiev. Transparent and competitive rates for effective customs support for your business. We make customs procedures affordable and profitable.</t>
+  </si>
+  <si>
     <t>price of customs services, cost of brokerage services, customs clearance tariffs, customs brokerage rates, customs services pricing policy, brokerage fees, customs clearance price, cost of customs brokerage services</t>
   </si>
   <si>
@@ -463,6 +523,9 @@
     <t>Customs Broker Kiev: Effective Customs Support for Your Business</t>
   </si>
   <si>
+    <t>Your reliable customs broker in Kyiv for international cargo operations. Optimize your customs procedures and ensure compliance with regulations with professional assistance. We make your international trade easier and more efficient</t>
+  </si>
+  <si>
     <t>export and import of goods, customs consulting, brokerage services for international trade, customs procedures, customs consultancy, customs consultant, brokerage services Kiev, customs fees, customs clearance of goods</t>
   </si>
   <si>
@@ -478,12 +541,12 @@
     <t>http://localhost:3000/en/blog/the-economics-of-low-cost-delivery-services</t>
   </si>
   <si>
-    <t xml:space="preserve">Low-cost air cargo delivery to Ukraine., Cost reduction , Increase in revenues </t>
-  </si>
-  <si>
     <t>The economics of low-cost delivery: how airlines are reducing costs and increasing revenues.</t>
   </si>
   <si>
+    <t>The economics of low-cost shipping: learn how airlines are reducing costs and increasing revenues through route optimization.</t>
+  </si>
+  <si>
     <t>economics of low-cost carriers, cargo delivery, cost reduction, revenue increase, route optimization, modern technologies in aviation, minimization of operating costs, airline competitiveness, low-cost carriers' strategies, air cargo operations</t>
   </si>
   <si>
@@ -496,6 +559,9 @@
     <t>Ways of transportation of containers from China to Ukraine</t>
   </si>
   <si>
+    <t>Learn about different ways of container transportation from China to Ukraine: sea, rail and multimodal transportation. Efficient logistics solutions for your business.</t>
+  </si>
+  <si>
     <t>ways of container delivery, types of container transportation, container transportation logistics, methods of container transportation, transportation of goods in containers, container transportation, container transportation options, efficient ways of container delivery</t>
   </si>
   <si>
@@ -505,12 +571,15 @@
     <t>http://localhost:3000/en/blog/how-to-write-an-inquiry-to-a-chinese-supplier</t>
   </si>
   <si>
-    <t>How to write a request to a Chinese supplier of goods?</t>
+    <t>How to write a inquiry to a Chinese supplier of goods? Detailed guide with examples.</t>
   </si>
   <si>
     <t>How to write a inquiry to a Chinese supplier of goods?</t>
   </si>
   <si>
+    <t>Detailed guide with examples. How to write a inquiry to a Chinese supplier of goods. A sample letter to a Chinese supplier.</t>
+  </si>
+  <si>
     <t>request to supplier, letter to seller, chinese suppliers, purchasing in china</t>
   </si>
   <si>
@@ -520,7 +589,7 @@
     <t>http://localhost:3000/en/blog/searching-for-suppliers-in-china</t>
   </si>
   <si>
-    <t>Searching for suppliers in China</t>
+    <t>Searching for suppliers in China, step-by-step instructions on how to find a supplier in China. Using alibaba.com as an example.</t>
   </si>
   <si>
     <t>Search for suppliers in China</t>
@@ -541,6 +610,9 @@
     <t>Ukraine's Customs Payments in August 2024 Reached 51.1 Billion UAH</t>
   </si>
   <si>
+    <t>In August 2024, customs payments of 51.1 billion UAH were directed to the state's revenue, which is 3.2 billion UAH more than the previous month. Find out what factors contributed to the increase.</t>
+  </si>
+  <si>
     <t>customs payments, Ukraine, August 2024, state budget, benefits, taxable imports</t>
   </si>
   <si>
@@ -550,6 +622,9 @@
     <t>Traffic Restrictions at the Hungarian Border for Two Weeks</t>
   </si>
   <si>
+    <t>Starting September 19, the Chop-Zahony crossing will have temporary traffic restrictions due to road repairs. Read more for details.</t>
+  </si>
+  <si>
     <t>border, Hungary, restrictions, Chop-Zahony, repair</t>
   </si>
   <si>
@@ -559,6 +634,9 @@
     <t>Cargo Ship Pallada Crashes Near Turkey: All Incident Details</t>
   </si>
   <si>
+    <t>Learn about the crash of the Pallada cargo ship, its consequences for the port and local residents.</t>
+  </si>
+  <si>
     <t>cargo ship Pallada, crash, Turkey, rescue operation, storm, consequences</t>
   </si>
   <si>
@@ -568,6 +646,9 @@
     <t>Corruption Scandal: Why MSC Refused to Enter Odessa</t>
   </si>
   <si>
+    <t>MSC canceled its entry into Odessa port due to corruption issues. How does this decision impact Ukraine and its economy?</t>
+  </si>
+  <si>
     <t>MSC, corruption, Odessa port, cargo delays, international logistics</t>
   </si>
   <si>
@@ -575,6 +656,9 @@
   </si>
   <si>
     <t>Odesa Ports Export Exceeded 60 Million Tons in 2024</t>
+  </si>
+  <si>
+    <t>Odesa ports exported over 60 million tons of goods in the first 11 months of 2024, despite attacks and challenging conditions, focusing on agricultural exports.</t>
   </si>
   <si>
     <t>Odesa, ports, export, agricultural products, grain, Ukraine, food security</t>
@@ -954,10 +1038,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:G56"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -976,24 +1060,27 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -1001,925 +1088,1063 @@
       <c r="F3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="G8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="G9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="G11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="G12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="G13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="F14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="G14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="E15" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="G15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="F16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="G16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="E17" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="F17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="G17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="E18" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="F18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="G18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="E19" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="F19" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="G19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="F20" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="G20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="C21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="E21" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="F21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="G21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="E22" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="F22" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="G22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="C23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="E23" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="F23" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="G23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="B24" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="E24" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="F24" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="G24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B25" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="E25" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="F25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="G25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B26" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="C26" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>10</v>
+        <v>113</v>
       </c>
       <c r="E26" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="F26" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="G26" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B27" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="C27" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>10</v>
+        <v>117</v>
       </c>
       <c r="E27" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="F27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="G27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="B28" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>121</v>
       </c>
       <c r="E28" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="F28" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="G28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="B29" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="C29" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="E29" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="F29" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="G29" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="B30" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="C30" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="E30" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="F30" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="G30" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="B31" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="C31" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D31" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="E31" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="F31" t="s">
+        <v>135</v>
+      </c>
+      <c r="G31" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>106</v>
-      </c>
       <c r="B32" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="C32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="E32" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="F32" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="G32" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="B33" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="C33" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="E33" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
       <c r="F33" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="G33" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="B34" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="C34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>10</v>
+        <v>147</v>
       </c>
       <c r="E34" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="F34" t="s">
-        <v>131</v>
+        <v>148</v>
+      </c>
+      <c r="G34" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B37" t="s">
-        <v>133</v>
+        <v>151</v>
       </c>
       <c r="C37" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="E37" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="F37" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+      <c r="G37" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B38" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="C38" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D38" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
       <c r="E38" t="s">
-        <v>139</v>
+        <v>156</v>
       </c>
       <c r="F38" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="G38" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B39" t="s">
-        <v>141</v>
+        <v>159</v>
       </c>
       <c r="C39" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D39" t="s">
-        <v>10</v>
+        <v>160</v>
       </c>
       <c r="E39" t="s">
-        <v>142</v>
+        <v>160</v>
       </c>
       <c r="F39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+      <c r="G39" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="B40" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D40" t="s">
-        <v>10</v>
+        <v>164</v>
       </c>
       <c r="E40" t="s">
-        <v>145</v>
+        <v>164</v>
       </c>
       <c r="F40" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+      <c r="G40" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="B41" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="C41" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D41" t="s">
-        <v>10</v>
+        <v>169</v>
       </c>
       <c r="E41" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="F41" t="s">
-        <v>150</v>
+        <v>170</v>
+      </c>
+      <c r="G41" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="B46" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="C46" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D46" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
       <c r="E46" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="F46" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+      <c r="G46" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="B47" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="C47" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D47" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
       <c r="E47" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
       <c r="F47" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+      <c r="G47" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="B48" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
       <c r="C48" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D48" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="E48" t="s">
-        <v>165</v>
+        <v>187</v>
       </c>
       <c r="F48" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="G48" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>167</v>
+        <v>190</v>
       </c>
       <c r="B49" t="s">
-        <v>168</v>
+        <v>191</v>
       </c>
       <c r="C49" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D49" t="s">
-        <v>169</v>
+        <v>192</v>
       </c>
       <c r="E49" t="s">
-        <v>170</v>
+        <v>193</v>
       </c>
       <c r="F49" t="s">
-        <v>171</v>
+        <v>192</v>
+      </c>
+      <c r="G49" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>173</v>
+        <v>196</v>
       </c>
       <c r="B52" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="C52" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D52" t="s">
-        <v>10</v>
+        <v>198</v>
       </c>
       <c r="E52" t="s">
-        <v>175</v>
+        <v>198</v>
       </c>
       <c r="F52" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="G52" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>173</v>
+        <v>196</v>
       </c>
       <c r="B53" t="s">
-        <v>177</v>
+        <v>201</v>
       </c>
       <c r="C53" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D53" t="s">
-        <v>10</v>
+        <v>202</v>
       </c>
       <c r="E53" t="s">
-        <v>178</v>
+        <v>202</v>
       </c>
       <c r="F53" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+      <c r="G53" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>173</v>
+        <v>196</v>
       </c>
       <c r="B54" t="s">
-        <v>180</v>
+        <v>205</v>
       </c>
       <c r="C54" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D54" t="s">
-        <v>10</v>
+        <v>206</v>
       </c>
       <c r="E54" t="s">
-        <v>181</v>
+        <v>206</v>
       </c>
       <c r="F54" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="G54" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>173</v>
+        <v>196</v>
       </c>
       <c r="B55" t="s">
-        <v>183</v>
+        <v>209</v>
       </c>
       <c r="C55" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D55" t="s">
-        <v>10</v>
+        <v>210</v>
       </c>
       <c r="E55" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="F55" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+      <c r="G55" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>173</v>
+        <v>196</v>
       </c>
       <c r="B56" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="C56" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D56" t="s">
-        <v>10</v>
+        <v>214</v>
       </c>
       <c r="E56" t="s">
-        <v>187</v>
+        <v>214</v>
       </c>
       <c r="F56" t="s">
-        <v>188</v>
+        <v>215</v>
+      </c>
+      <c r="G56" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>